<commit_message>
updated project tracking matrix
</commit_message>
<xml_diff>
--- a/Management Plan/Project Tracking Matrix.xlsx
+++ b/Management Plan/Project Tracking Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CECS 491A\491Project\Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E978CAE1-40CE-4907-B79E-3FEC7BE43274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80120E77-3879-4E71-AD73-192EEB58EA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D06805A4-F894-45EA-900A-1FB3C4089801}"/>
+    <workbookView xWindow="17475" yWindow="3615" windowWidth="21600" windowHeight="11385" xr2:uid="{D06805A4-F894-45EA-900A-1FB3C4089801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="87">
   <si>
     <t>Project Tracking Matrix</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>SCOPE STATEMENT</t>
-  </si>
-  <si>
-    <t>Sprint #0 - Sprint Planning, PrelimBRDPresentation, BRD, MP</t>
   </si>
   <si>
     <t>AT RISK</t>
@@ -191,13 +188,112 @@
     <t>MP - Sprint Restrospective</t>
   </si>
   <si>
-    <t>MP - Sprint Review Records</t>
-  </si>
-  <si>
     <t>StudiBuddi</t>
   </si>
   <si>
     <t>StudiBuddi will allow students to connect with other students to help each other get help in similar courses, develop studying habits, and expand their network amongst students</t>
+  </si>
+  <si>
+    <t>Sprint #1 - Sprint Planning, PRD, ADD, update BRD, database design</t>
+  </si>
+  <si>
+    <t>PRD - Goals</t>
+  </si>
+  <si>
+    <t>PRD</t>
+  </si>
+  <si>
+    <t>User Personas</t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>Server Sitemap</t>
+  </si>
+  <si>
+    <t>Page Description</t>
+  </si>
+  <si>
+    <t>Tanner M. &amp; Hunter D.</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Additional Functional Requirements</t>
+  </si>
+  <si>
+    <t>Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>Performance Requirements</t>
+  </si>
+  <si>
+    <t>Future Iterations</t>
+  </si>
+  <si>
+    <t>API Diagram</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>Languages Diagram</t>
+  </si>
+  <si>
+    <t>Deployment Diagram</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Use case diagram</t>
+  </si>
+  <si>
+    <t>Activity diagram</t>
+  </si>
+  <si>
+    <t>Tradeoff Analysis - Mobile vs. web</t>
+  </si>
+  <si>
+    <t>Tradeoff Analysis - Android vs. iOS</t>
+  </si>
+  <si>
+    <t>Tradeoff Analysis - Database</t>
+  </si>
+  <si>
+    <t>Risk Management</t>
+  </si>
+  <si>
+    <t>Sprint 1 Planning Meeting</t>
+  </si>
+  <si>
+    <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Update BRD</t>
+  </si>
+  <si>
+    <t>Tymee K. &amp; Luke K.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Implement Database</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Tanner M. &amp; Oscar G.</t>
   </si>
 </sst>
 </file>
@@ -311,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -384,9 +480,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0389D8-26FB-4715-9BE6-5F5BE54600CD}">
   <dimension ref="A1:AE984"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -779,7 +872,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="4"/>
@@ -806,10 +899,10 @@
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="12">
         <v>43852</v>
@@ -826,7 +919,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="4"/>
@@ -885,34 +978,34 @@
     <row r="5" spans="1:31" ht="39" thickBot="1">
       <c r="A5" s="6"/>
       <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -939,7 +1032,7 @@
       <c r="A6" s="6"/>
       <c r="B6" s="17"/>
       <c r="C6" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -954,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="4"/>
@@ -982,13 +1075,13 @@
       <c r="A7" s="6"/>
       <c r="B7" s="20"/>
       <c r="C7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="F7" s="21">
         <v>3</v>
@@ -1003,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="4"/>
@@ -1027,17 +1120,17 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
     </row>
-    <row r="8" spans="1:31" ht="41.25" thickBot="1">
+    <row r="8" spans="1:31" ht="27.75" thickBot="1">
       <c r="A8" s="6"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="21">
         <v>5</v>
@@ -1052,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="4"/>
@@ -1076,16 +1169,16 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
     </row>
-    <row r="9" spans="1:31" ht="27.75" thickBot="1">
+    <row r="9" spans="1:31" ht="16.5" thickBot="1">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>7</v>
@@ -1103,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="4"/>
@@ -1130,16 +1223,16 @@
     <row r="10" spans="1:31" ht="27.75" thickBot="1">
       <c r="A10" s="6"/>
       <c r="B10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>32</v>
       </c>
       <c r="F10" s="21">
         <v>3</v>
@@ -1154,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" s="21"/>
       <c r="L10" s="4"/>
@@ -1178,17 +1271,17 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
     </row>
-    <row r="11" spans="1:31" ht="54.75" thickBot="1">
+    <row r="11" spans="1:31" ht="27.75" thickBot="1">
       <c r="A11" s="6"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="21">
         <v>2</v>
@@ -1203,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="21"/>
       <c r="L11" s="4"/>
@@ -1227,14 +1320,14 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
     </row>
-    <row r="12" spans="1:31" ht="68.25" thickBot="1">
+    <row r="12" spans="1:31" ht="41.25" thickBot="1">
       <c r="A12" s="6"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>7</v>
@@ -1252,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12" s="4"/>
@@ -1276,17 +1369,17 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
     </row>
-    <row r="13" spans="1:31" ht="81.75" thickBot="1">
+    <row r="13" spans="1:31" ht="54.75" thickBot="1">
       <c r="A13" s="6"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="F13" s="21">
         <v>5</v>
@@ -1301,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="4"/>
@@ -1325,17 +1418,17 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:31" ht="41.25" thickBot="1">
+    <row r="14" spans="1:31" ht="27.75" thickBot="1">
       <c r="A14" s="6"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="F14" s="21">
         <v>3</v>
@@ -1350,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K14" s="21"/>
       <c r="L14" s="4"/>
@@ -1374,19 +1467,19 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:31" ht="68.25" thickBot="1">
+    <row r="15" spans="1:31" ht="41.25" thickBot="1">
       <c r="A15" s="6"/>
       <c r="B15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="21">
         <v>3</v>
@@ -1401,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="4"/>
@@ -1425,16 +1518,16 @@
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
     </row>
-    <row r="16" spans="1:31" ht="41.25" thickBot="1">
+    <row r="16" spans="1:31" ht="27.75" thickBot="1">
       <c r="A16" s="6"/>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>7</v>
@@ -1452,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K16" s="21"/>
       <c r="L16" s="4"/>
@@ -1476,17 +1569,17 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
     </row>
-    <row r="17" spans="1:31" ht="41.25" thickBot="1">
+    <row r="17" spans="1:31" ht="27.75" thickBot="1">
       <c r="A17" s="6"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>42</v>
       </c>
       <c r="F17" s="21">
         <v>3</v>
@@ -1501,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K17" s="21"/>
       <c r="L17" s="4"/>
@@ -1525,19 +1618,19 @@
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
     </row>
-    <row r="18" spans="1:31" ht="41.25" thickBot="1">
+    <row r="18" spans="1:31" ht="27.75" thickBot="1">
       <c r="A18" s="6"/>
       <c r="B18" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="F18" s="21">
         <v>5</v>
@@ -1552,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" s="21"/>
       <c r="L18" s="4"/>
@@ -1576,17 +1669,17 @@
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
     </row>
-    <row r="19" spans="1:31" ht="41.25" thickBot="1">
+    <row r="19" spans="1:31" ht="27.75" thickBot="1">
       <c r="A19" s="6"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="21">
         <v>3</v>
@@ -1601,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K19" s="21"/>
       <c r="L19" s="4"/>
@@ -1625,14 +1718,14 @@
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
     </row>
-    <row r="20" spans="1:31" ht="41.25" thickBot="1">
+    <row r="20" spans="1:31" ht="27.75" thickBot="1">
       <c r="A20" s="6"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>7</v>
@@ -1650,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K20" s="21"/>
       <c r="L20" s="4"/>
@@ -1674,17 +1767,17 @@
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
     </row>
-    <row r="21" spans="1:31" ht="54.75" thickBot="1">
+    <row r="21" spans="1:31" ht="41.25" thickBot="1">
       <c r="A21" s="6"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="21">
         <v>5</v>
@@ -1699,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K21" s="21"/>
       <c r="L21" s="4"/>
@@ -1723,14 +1816,14 @@
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
     </row>
-    <row r="22" spans="1:31" ht="41.25" thickBot="1">
+    <row r="22" spans="1:31" ht="27.75" thickBot="1">
       <c r="A22" s="6"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>7</v>
@@ -1748,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K22" s="21"/>
       <c r="L22" s="4"/>
@@ -1776,13 +1869,13 @@
       <c r="A23" s="6"/>
       <c r="B23" s="20"/>
       <c r="C23" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="21">
         <v>3</v>
@@ -1797,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="21"/>
       <c r="L23" s="4"/>
@@ -1821,17 +1914,17 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
     </row>
-    <row r="24" spans="1:31" ht="54.75" thickBot="1">
+    <row r="24" spans="1:31" ht="41.25" thickBot="1">
       <c r="A24" s="6"/>
       <c r="B24" s="20"/>
       <c r="C24" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="21">
         <v>5</v>
@@ -1846,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24" s="21"/>
       <c r="L24" s="4"/>
@@ -1870,32 +1963,32 @@
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
     </row>
-    <row r="25" spans="1:31" ht="54.75" thickBot="1">
+    <row r="25" spans="1:31" ht="16.5" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="20"/>
       <c r="C25" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F25" s="21">
         <v>5</v>
       </c>
       <c r="G25" s="22">
-        <v>43877</v>
+        <v>43897</v>
       </c>
       <c r="H25" s="22">
-        <v>43877</v>
+        <v>43897</v>
       </c>
       <c r="I25" s="21">
         <v>0</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K25" s="21"/>
       <c r="L25" s="4"/>
@@ -1919,18 +2012,34 @@
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
     </row>
-    <row r="26" spans="1:31" ht="15.75">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+    <row r="26" spans="1:31" ht="16.5" thickBot="1">
+      <c r="A26" s="6"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="21">
+        <v>5</v>
+      </c>
+      <c r="G26" s="22">
+        <v>43897</v>
+      </c>
+      <c r="H26" s="22">
+        <v>43900</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="21"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -1952,18 +2061,34 @@
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
     </row>
-    <row r="27" spans="1:31" ht="15.75">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+    <row r="27" spans="1:31" ht="16.5" thickBot="1">
+      <c r="A27" s="6"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="21">
+        <v>5</v>
+      </c>
+      <c r="G27" s="22">
+        <v>43898</v>
+      </c>
+      <c r="H27" s="22">
+        <v>43902</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="21"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1985,18 +2110,34 @@
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
     </row>
-    <row r="28" spans="1:31" ht="15.75">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+    <row r="28" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A28" s="6"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="21">
+        <v>5</v>
+      </c>
+      <c r="G28" s="22">
+        <v>43897</v>
+      </c>
+      <c r="H28" s="22">
+        <v>43897</v>
+      </c>
+      <c r="I28" s="21">
+        <v>0</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="21"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -2018,18 +2159,34 @@
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
     </row>
-    <row r="29" spans="1:31" ht="15.75">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+    <row r="29" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A29" s="6"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="21">
+        <v>5</v>
+      </c>
+      <c r="G29" s="22">
+        <v>43897</v>
+      </c>
+      <c r="H29" s="22">
+        <v>43897</v>
+      </c>
+      <c r="I29" s="21">
+        <v>0</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="21"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2051,18 +2208,34 @@
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
     </row>
-    <row r="30" spans="1:31" ht="15.75">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+    <row r="30" spans="1:31" ht="16.5" thickBot="1">
+      <c r="A30" s="6"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="21">
+        <v>5</v>
+      </c>
+      <c r="G30" s="22">
+        <v>43897</v>
+      </c>
+      <c r="H30" s="22">
+        <v>43902</v>
+      </c>
+      <c r="I30" s="21">
+        <v>0</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="21"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2084,18 +2257,34 @@
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
     </row>
-    <row r="31" spans="1:31" ht="15.75">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+    <row r="31" spans="1:31" ht="16.5" thickBot="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="21">
+        <v>5</v>
+      </c>
+      <c r="G31" s="22">
+        <v>43897</v>
+      </c>
+      <c r="H31" s="22">
+        <v>43897</v>
+      </c>
+      <c r="I31" s="21">
+        <v>0</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="21"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2117,18 +2306,34 @@
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
     </row>
-    <row r="32" spans="1:31" ht="15.75">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+    <row r="32" spans="1:31" ht="41.25" thickBot="1">
+      <c r="A32" s="6"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="21">
+        <v>5</v>
+      </c>
+      <c r="G32" s="22">
+        <v>43898</v>
+      </c>
+      <c r="H32" s="22">
+        <v>43902</v>
+      </c>
+      <c r="I32" s="21">
+        <v>0</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="21"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2150,18 +2355,34 @@
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
     </row>
-    <row r="33" spans="1:31" ht="15.75">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+    <row r="33" spans="1:31" ht="41.25" thickBot="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="21">
+        <v>5</v>
+      </c>
+      <c r="G33" s="22">
+        <v>43898</v>
+      </c>
+      <c r="H33" s="22">
+        <v>43902</v>
+      </c>
+      <c r="I33" s="21">
+        <v>0</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="21"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2183,18 +2404,34 @@
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
     </row>
-    <row r="34" spans="1:31" ht="15.75">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+    <row r="34" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="21">
+        <v>5</v>
+      </c>
+      <c r="G34" s="22">
+        <v>43898</v>
+      </c>
+      <c r="H34" s="22">
+        <v>43900</v>
+      </c>
+      <c r="I34" s="21">
+        <v>0</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="21"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2216,18 +2453,34 @@
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
     </row>
-    <row r="35" spans="1:31" ht="15.75">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+    <row r="35" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A35" s="6"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="21">
+        <v>5</v>
+      </c>
+      <c r="G35" s="22">
+        <v>43898</v>
+      </c>
+      <c r="H35" s="22">
+        <v>43902</v>
+      </c>
+      <c r="I35" s="21">
+        <v>0</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="21"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2249,18 +2502,34 @@
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
     </row>
-    <row r="36" spans="1:31" ht="15.75">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+    <row r="36" spans="1:31" ht="16.5" thickBot="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="21">
+        <v>5</v>
+      </c>
+      <c r="G36" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H36" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I36" s="21">
+        <v>0</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="21"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -2282,18 +2551,34 @@
       <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
     </row>
-    <row r="37" spans="1:31" ht="15.75">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+    <row r="37" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A37" s="6"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="21">
+        <v>5</v>
+      </c>
+      <c r="G37" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H37" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I37" s="21">
+        <v>0</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="21"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -2315,18 +2600,34 @@
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
     </row>
-    <row r="38" spans="1:31" ht="15.75">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+    <row r="38" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A38" s="6"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="21">
+        <v>5</v>
+      </c>
+      <c r="G38" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H38" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I38" s="21">
+        <v>0</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="21"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -2348,18 +2649,34 @@
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
     </row>
-    <row r="39" spans="1:31" ht="15.75">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+    <row r="39" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A39" s="6"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="21">
+        <v>5</v>
+      </c>
+      <c r="G39" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H39" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I39" s="21">
+        <v>0</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="21"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -2381,18 +2698,34 @@
       <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
     </row>
-    <row r="40" spans="1:31" ht="15.75">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+    <row r="40" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A40" s="6"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="21">
+        <v>5</v>
+      </c>
+      <c r="G40" s="22">
+        <v>43905</v>
+      </c>
+      <c r="H40" s="22">
+        <v>43905</v>
+      </c>
+      <c r="I40" s="21">
+        <v>0</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="21"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -2414,18 +2747,34 @@
       <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
     </row>
-    <row r="41" spans="1:31" ht="15.75">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+    <row r="41" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A41" s="6"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="21">
+        <v>5</v>
+      </c>
+      <c r="G41" s="22">
+        <v>43905</v>
+      </c>
+      <c r="H41" s="22">
+        <v>43905</v>
+      </c>
+      <c r="I41" s="21">
+        <v>0</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" s="21"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -2447,18 +2796,34 @@
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
     </row>
-    <row r="42" spans="1:31" ht="15.75">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+    <row r="42" spans="1:31" ht="54.75" thickBot="1">
+      <c r="A42" s="6"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="21">
+        <v>5</v>
+      </c>
+      <c r="G42" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H42" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I42" s="21">
+        <v>0</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="21"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -2480,18 +2845,34 @@
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
     </row>
-    <row r="43" spans="1:31" ht="15.75">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+    <row r="43" spans="1:31" ht="54.75" thickBot="1">
+      <c r="A43" s="6"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="21">
+        <v>5</v>
+      </c>
+      <c r="G43" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H43" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I43" s="21">
+        <v>0</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" s="21"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
@@ -2513,28 +2894,44 @@
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
     </row>
-    <row r="44" spans="1:31" ht="15.75">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
+    <row r="44" spans="1:31" ht="41.25" thickBot="1">
+      <c r="A44" s="6"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="21">
+        <v>5</v>
+      </c>
+      <c r="G44" s="22">
+        <v>43904</v>
+      </c>
+      <c r="H44" s="22">
+        <v>43904</v>
+      </c>
+      <c r="I44" s="21">
+        <v>0</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="21"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
       <c r="X44" s="4"/>
@@ -2546,18 +2943,34 @@
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
     </row>
-    <row r="45" spans="1:31" ht="15.75">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
+    <row r="45" spans="1:31" ht="41.25" thickBot="1">
+      <c r="A45" s="6"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="21">
+        <v>5</v>
+      </c>
+      <c r="G45" s="22">
+        <v>43905</v>
+      </c>
+      <c r="H45" s="22">
+        <v>43905</v>
+      </c>
+      <c r="I45" s="21">
+        <v>0</v>
+      </c>
+      <c r="J45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="21"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -2579,28 +2992,44 @@
       <c r="AD45" s="5"/>
       <c r="AE45" s="5"/>
     </row>
-    <row r="46" spans="1:31" ht="15.75">
-      <c r="A46" s="5"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+    <row r="46" spans="1:31" ht="41.25" thickBot="1">
+      <c r="A46" s="6"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="21">
+        <v>5</v>
+      </c>
+      <c r="G46" s="22">
+        <v>43885</v>
+      </c>
+      <c r="H46" s="22">
+        <v>43885</v>
+      </c>
+      <c r="I46" s="21">
+        <v>0</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="21"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
       <c r="X46" s="4"/>
@@ -2612,28 +3041,44 @@
       <c r="AD46" s="4"/>
       <c r="AE46" s="4"/>
     </row>
-    <row r="47" spans="1:31" ht="15.75">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
+    <row r="47" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A47" s="6"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="21">
+        <v>5</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I47" s="21">
+        <v>0</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="K47" s="21"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
@@ -2645,28 +3090,44 @@
       <c r="AD47" s="4"/>
       <c r="AE47" s="4"/>
     </row>
-    <row r="48" spans="1:31" ht="15.75">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
+    <row r="48" spans="1:31" ht="27.75" thickBot="1">
+      <c r="A48" s="6"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" s="21">
+        <v>5</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I48" s="21">
+        <v>0</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="K48" s="21"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
@@ -2681,25 +3142,25 @@
     <row r="49" spans="1:31" ht="15.75">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
@@ -2714,25 +3175,25 @@
     <row r="50" spans="1:31" ht="15.75">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
       <c r="V50" s="4"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>
@@ -2747,25 +3208,25 @@
     <row r="51" spans="1:31" ht="15.75">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
       <c r="X51" s="4"/>
@@ -2780,25 +3241,25 @@
     <row r="52" spans="1:31" ht="15.75">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
-      <c r="U52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
       <c r="V52" s="4"/>
       <c r="W52" s="4"/>
       <c r="X52" s="4"/>
@@ -2813,25 +3274,25 @@
     <row r="53" spans="1:31" ht="15.75">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
       <c r="X53" s="4"/>
@@ -2846,25 +3307,25 @@
     <row r="54" spans="1:31" ht="15.75">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
       <c r="V54" s="4"/>
       <c r="W54" s="4"/>
       <c r="X54" s="4"/>
@@ -2879,25 +3340,25 @@
     <row r="55" spans="1:31" ht="15.75">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
       <c r="V55" s="4"/>
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
@@ -2912,25 +3373,25 @@
     <row r="56" spans="1:31" ht="15.75">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
       <c r="V56" s="4"/>
       <c r="W56" s="4"/>
       <c r="X56" s="4"/>
@@ -2945,25 +3406,25 @@
     <row r="57" spans="1:31" ht="15.75">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
       <c r="V57" s="4"/>
       <c r="W57" s="4"/>
       <c r="X57" s="4"/>
@@ -2978,25 +3439,25 @@
     <row r="58" spans="1:31" ht="15.75">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
       <c r="V58" s="4"/>
       <c r="W58" s="4"/>
       <c r="X58" s="4"/>
@@ -3011,25 +3472,25 @@
     <row r="59" spans="1:31" ht="15.75">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
       <c r="V59" s="4"/>
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
@@ -3044,25 +3505,25 @@
     <row r="60" spans="1:31" ht="15.75">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5"/>
       <c r="V60" s="4"/>
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
@@ -3077,25 +3538,25 @@
     <row r="61" spans="1:31" ht="15.75">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
       <c r="V61" s="4"/>
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
@@ -3110,25 +3571,25 @@
     <row r="62" spans="1:31" ht="15.75">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
-      <c r="U62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
       <c r="V62" s="4"/>
       <c r="W62" s="4"/>
       <c r="X62" s="4"/>
@@ -3143,25 +3604,25 @@
     <row r="63" spans="1:31" ht="15.75">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-      <c r="U63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
       <c r="V63" s="4"/>
       <c r="W63" s="4"/>
       <c r="X63" s="4"/>
@@ -3176,25 +3637,25 @@
     <row r="64" spans="1:31" ht="15.75">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-      <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
-      <c r="U64" s="4"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="5"/>
       <c r="V64" s="4"/>
       <c r="W64" s="4"/>
       <c r="X64" s="4"/>
@@ -3209,25 +3670,25 @@
     <row r="65" spans="1:31" ht="15.75">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-      <c r="U65" s="4"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="5"/>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="T65" s="5"/>
+      <c r="U65" s="5"/>
       <c r="V65" s="4"/>
       <c r="W65" s="4"/>
       <c r="X65" s="4"/>
@@ -3242,25 +3703,25 @@
     <row r="66" spans="1:31" ht="15.75">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
       <c r="V66" s="4"/>
       <c r="W66" s="4"/>
       <c r="X66" s="4"/>
@@ -3275,25 +3736,25 @@
     <row r="67" spans="1:31" ht="15.75">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
-      <c r="U67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
       <c r="V67" s="4"/>
       <c r="W67" s="4"/>
       <c r="X67" s="4"/>
@@ -3308,25 +3769,25 @@
     <row r="68" spans="1:31" ht="15.75">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
-      <c r="U68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="5"/>
       <c r="V68" s="4"/>
       <c r="W68" s="4"/>
       <c r="X68" s="4"/>
@@ -33567,9 +34028,6 @@
       <c r="AE984" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B46:K46"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>